<commit_message>
use pathologyID in all metadata files
</commit_message>
<xml_diff>
--- a/Documentation/samples.xlsx
+++ b/Documentation/samples.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">sampleID</t>
   </si>
   <si>
-    <t xml:space="preserve">pathology</t>
+    <t xml:space="preserve">pathologyID</t>
   </si>
   <si>
     <t xml:space="preserve">Causal gene</t>
@@ -206,15 +206,15 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
samples.xlsx : add Sex column
</commit_message>
<xml_diff>
--- a/Documentation/samples.xlsx
+++ b/Documentation/samples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">specimenID</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">sampleID</t>
   </si>
   <si>
+    <t xml:space="preserve">Sex</t>
+  </si>
+  <si>
     <t xml:space="preserve">pathologyID</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">grexome0001</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">MMAF</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">grexome0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">Ovo</t>
@@ -203,18 +212,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="12.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,62 +239,74 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>